<commit_message>
SAE 303 - Update datasets
</commit_message>
<xml_diff>
--- a/integration-web-s3/sae-303/datasets/crea/choix-parcours-s3-mmi-2023.xlsx
+++ b/integration-web-s3/sae-303/datasets/crea/choix-parcours-s3-mmi-2023.xlsx
@@ -588,7 +588,7 @@
         <v>14</v>
       </c>
       <c r="K2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L2">
         <v>10</v>
@@ -597,7 +597,7 @@
         <v>11</v>
       </c>
       <c r="N2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O2">
         <v>6</v>
@@ -609,22 +609,22 @@
         <v>7</v>
       </c>
       <c r="R2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T2">
         <v>7</v>
       </c>
       <c r="U2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="V2">
         <v>5</v>
       </c>
       <c r="W2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="X2">
         <v>1</v>
@@ -633,13 +633,13 @@
         <v>4</v>
       </c>
       <c r="Z2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AA2">
         <v>9</v>
       </c>
       <c r="AB2">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:28">
@@ -647,16 +647,16 @@
         <v>29</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -665,13 +665,13 @@
         <v>3</v>
       </c>
       <c r="H3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K3">
         <v>13</v>
@@ -763,13 +763,13 @@
         <v>4</v>
       </c>
       <c r="L4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M4">
         <v>3</v>
       </c>
       <c r="N4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O4">
         <v>1</v>
@@ -778,16 +778,16 @@
         <v>2</v>
       </c>
       <c r="Q4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R4">
         <v>1</v>
       </c>
       <c r="S4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="T4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="U4">
         <v>7</v>
@@ -796,7 +796,7 @@
         <v>14</v>
       </c>
       <c r="W4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X4">
         <v>8</v>
@@ -808,10 +808,10 @@
         <v>7</v>
       </c>
       <c r="AA4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB4">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>